<commit_message>
New_files and potential solution to the time error
</commit_message>
<xml_diff>
--- a/VO2_excel.xlsx
+++ b/VO2_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Holash\Documents\Knes381\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875E67DF-4D23-4D06-B9C7-4FC811778500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99712D9D-31E1-4886-A0FE-8898BB56EF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18396" yWindow="2808" windowWidth="22080" windowHeight="23268" xr2:uid="{44229B90-BAE9-457D-BDB1-1FF2291576CF}"/>
+    <workbookView xWindow="5520" yWindow="2328" windowWidth="37536" windowHeight="23508" xr2:uid="{44229B90-BAE9-457D-BDB1-1FF2291576CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -483,7 +505,7 @@
   <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N2"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3413,5 +3435,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>